<commit_message>
Testes unitarios TipoUsuarioService, UsuarioService
</commit_message>
<xml_diff>
--- a/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
+++ b/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c20d8aba5601db01/Documentos/00_DigitalHouse/06_BACKEND/00_trabalho_em_Grupo/dentalclinic/dentalclinic/src/test/java/br/com/dentalclinic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9639BDF-7AF2-4B47-8416-FBF1B2A4ACCB}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEDB455-E3C3-4F57-B727-70AA9495471A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EE38068E-1540-4545-93C9-0DD6012C8E13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE38068E-1540-4545-93C9-0DD6012C8E13}"/>
   </bookViews>
   <sheets>
     <sheet name="GeraEndereco" sheetId="3" r:id="rId1"/>
     <sheet name="Clinica" sheetId="4" r:id="rId2"/>
+    <sheet name="Usuario" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="169">
   <si>
     <t>logradouro</t>
   </si>
@@ -444,6 +467,105 @@
   </si>
   <si>
     <t>Clinica Mega Popular</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>chars</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>TipoUsuario</t>
+  </si>
+  <si>
+    <t>Dentista</t>
+  </si>
+  <si>
+    <t>Recepcionista</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Administrador</t>
   </si>
 </sst>
 </file>
@@ -1711,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1444F6DF-8D46-41DE-AE9D-18B86BE86F24}">
   <dimension ref="C1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
@@ -1927,4 +2049,574 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D6BEF-0063-487A-8FD9-30F4346C7EFC}">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f ca="1">B2&amp;";"&amp;C2&amp;";"&amp;D2</f>
+        <v>sgtbpsscharsv@pprovicer.com.br;sgtbpsscharsv;Administrador</v>
+      </c>
+      <c r="B2" t="str">
+        <f ca="1">C2&amp;"@pprovicer.com.br"</f>
+        <v>sgtbpsscharsv@pprovicer.com.br</v>
+      </c>
+      <c r="C2" t="str" cm="1">
+        <f t="array" aca="1" ref="C2" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>sgtbpsscharsv</v>
+      </c>
+      <c r="D2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f t="shared" ref="A3:A28" ca="1" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3</f>
+        <v>tyarrqbvm@pprovicer.com.br;tyarrqbvm;Dentista</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B28" ca="1" si="1">C3&amp;"@pprovicer.com.br"</f>
+        <v>tyarrqbvm@pprovicer.com.br</v>
+      </c>
+      <c r="C3" t="str" cm="1">
+        <f t="array" aca="1" ref="C3" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>tyarrqbvm</v>
+      </c>
+      <c r="D3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>glqopbqschars@pprovicer.com.br;glqopbqschars;Recepcionista</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>glqopbqschars@pprovicer.com.br</v>
+      </c>
+      <c r="C4" t="str" cm="1">
+        <f t="array" aca="1" ref="C4" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>glqopbqschars</v>
+      </c>
+      <c r="D4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>charsajntfhcs@pprovicer.com.br;charsajntfhcs;Paciente</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>charsajntfhcs@pprovicer.com.br</v>
+      </c>
+      <c r="C5" t="str" cm="1">
+        <f t="array" aca="1" ref="C5" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>charsajntfhcs</v>
+      </c>
+      <c r="D5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>umjccharsrjuo@pprovicer.com.br;umjccharsrjuo;Administrador</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>umjccharsrjuo@pprovicer.com.br</v>
+      </c>
+      <c r="C6" t="str" cm="1">
+        <f t="array" aca="1" ref="C6" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>umjccharsrjuo</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
+      </c>
+      <c r="G6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>ukiqjxhfe@pprovicer.com.br;ukiqjxhfe;Dentista</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>ukiqjxhfe@pprovicer.com.br</v>
+      </c>
+      <c r="C7" t="str" cm="1">
+        <f t="array" aca="1" ref="C7" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>ukiqjxhfe</v>
+      </c>
+      <c r="D7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>shmjtacharsur@pprovicer.com.br;shmjtacharsur;Recepcionista</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>shmjtacharsur@pprovicer.com.br</v>
+      </c>
+      <c r="C8" t="str" cm="1">
+        <f t="array" aca="1" ref="C8" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>shmjtacharsur</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="G8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>orcharslxboul@pprovicer.com.br;orcharslxboul;Paciente</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>orcharslxboul@pprovicer.com.br</v>
+      </c>
+      <c r="C9" t="str" cm="1">
+        <f t="array" aca="1" ref="C9" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>orcharslxboul</v>
+      </c>
+      <c r="D9" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>jvmxcharsmvle@pprovicer.com.br;jvmxcharsmvle;Administrador</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>jvmxcharsmvle@pprovicer.com.br</v>
+      </c>
+      <c r="C10" t="str" cm="1">
+        <f t="array" aca="1" ref="C10" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>jvmxcharsmvle</v>
+      </c>
+      <c r="D10" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>oaeratyoe@pprovicer.com.br;oaeratyoe;Dentista</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>oaeratyoe@pprovicer.com.br</v>
+      </c>
+      <c r="C11" t="str" cm="1">
+        <f t="array" aca="1" ref="C11" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>oaeratyoe</v>
+      </c>
+      <c r="D11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>charsuxyjvidb@pprovicer.com.br;charsuxyjvidb;Recepcionista</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>charsuxyjvidb@pprovicer.com.br</v>
+      </c>
+      <c r="C12" t="str" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>charsuxyjvidb</v>
+      </c>
+      <c r="D12" t="s">
+        <v>166</v>
+      </c>
+      <c r="G12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>cjohjyumk@pprovicer.com.br;cjohjyumk;Paciente</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>cjohjyumk@pprovicer.com.br</v>
+      </c>
+      <c r="C13" t="str" cm="1">
+        <f t="array" aca="1" ref="C13" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>cjohjyumk</v>
+      </c>
+      <c r="D13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>tespcxhcb@pprovicer.com.br;tespcxhcb;Administrador</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>tespcxhcb@pprovicer.com.br</v>
+      </c>
+      <c r="C14" t="str" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>tespcxhcb</v>
+      </c>
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>rcharsvmuqtrf@pprovicer.com.br;rcharsvmuqtrf;Dentista</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>rcharsvmuqtrf@pprovicer.com.br</v>
+      </c>
+      <c r="C15" t="str" cm="1">
+        <f t="array" aca="1" ref="C15" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>rcharsvmuqtrf</v>
+      </c>
+      <c r="D15" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>gegheenbchars@pprovicer.com.br;gegheenbchars;Recepcionista</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>gegheenbchars@pprovicer.com.br</v>
+      </c>
+      <c r="C16" t="str" cm="1">
+        <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>gegheenbchars</v>
+      </c>
+      <c r="D16" t="s">
+        <v>166</v>
+      </c>
+      <c r="G16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>oagacharsxbjg@pprovicer.com.br;oagacharsxbjg;Paciente</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>oagacharsxbjg@pprovicer.com.br</v>
+      </c>
+      <c r="C17" t="str" cm="1">
+        <f t="array" aca="1" ref="C17" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>oagacharsxbjg</v>
+      </c>
+      <c r="D17" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>jibbvxgfl@pprovicer.com.br;jibbvxgfl;Administrador</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>jibbvxgfl@pprovicer.com.br</v>
+      </c>
+      <c r="C18" t="str" cm="1">
+        <f t="array" aca="1" ref="C18" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>jibbvxgfl</v>
+      </c>
+      <c r="D18" t="s">
+        <v>168</v>
+      </c>
+      <c r="G18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>charsstihrxlu@pprovicer.com.br;charsstihrxlu;Dentista</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>charsstihrxlu@pprovicer.com.br</v>
+      </c>
+      <c r="C19" t="str" cm="1">
+        <f t="array" aca="1" ref="C19" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>charsstihrxlu</v>
+      </c>
+      <c r="D19" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>kaphjyucharsb@pprovicer.com.br;kaphjyucharsb;Recepcionista</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>kaphjyucharsb@pprovicer.com.br</v>
+      </c>
+      <c r="C20" t="str" cm="1">
+        <f t="array" aca="1" ref="C20" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>kaphjyucharsb</v>
+      </c>
+      <c r="D20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>puvbktlre@pprovicer.com.br;puvbktlre;Paciente</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>puvbktlre@pprovicer.com.br</v>
+      </c>
+      <c r="C21" t="str" cm="1">
+        <f t="array" aca="1" ref="C21" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>puvbktlre</v>
+      </c>
+      <c r="D21" t="s">
+        <v>167</v>
+      </c>
+      <c r="G21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>uojjdgjvc@pprovicer.com.br;uojjdgjvc;Administrador</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>uojjdgjvc@pprovicer.com.br</v>
+      </c>
+      <c r="C22" t="str" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>uojjdgjvc</v>
+      </c>
+      <c r="D22" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>draohjsve@pprovicer.com.br;draohjsve;Dentista</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>draohjsve@pprovicer.com.br</v>
+      </c>
+      <c r="C23" t="str" cm="1">
+        <f t="array" aca="1" ref="C23" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>draohjsve</v>
+      </c>
+      <c r="D23" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>qyfsrdoqchars@pprovicer.com.br;qyfsrdoqchars;Recepcionista</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>qyfsrdoqchars@pprovicer.com.br</v>
+      </c>
+      <c r="C24" t="str" cm="1">
+        <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>qyfsrdoqchars</v>
+      </c>
+      <c r="D24" t="s">
+        <v>166</v>
+      </c>
+      <c r="G24" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>charscqnvinxt@pprovicer.com.br;charscqnvinxt;Paciente</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>charscqnvinxt@pprovicer.com.br</v>
+      </c>
+      <c r="C25" t="str" cm="1">
+        <f t="array" aca="1" ref="C25" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>charscqnvinxt</v>
+      </c>
+      <c r="D25" t="s">
+        <v>167</v>
+      </c>
+      <c r="G25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>fecharsnojgnchars@pprovicer.com.br;fecharsnojgnchars;Administrador</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>fecharsnojgnchars@pprovicer.com.br</v>
+      </c>
+      <c r="C26" t="str" cm="1">
+        <f t="array" aca="1" ref="C26" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>fecharsnojgnchars</v>
+      </c>
+      <c r="D26" t="s">
+        <v>168</v>
+      </c>
+      <c r="G26" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lgevkrkfm@pprovicer.com.br;lgevkrkfm;Dentista</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>lgevkrkfm@pprovicer.com.br</v>
+      </c>
+      <c r="C27" t="str" cm="1">
+        <f t="array" aca="1" ref="C27" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>lgevkrkfm</v>
+      </c>
+      <c r="D27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>charsbckavmls@pprovicer.com.br;charsbckavmls;Recepcionista</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>charsbckavmls@pprovicer.com.br</v>
+      </c>
+      <c r="C28" t="str" cm="1">
+        <f t="array" aca="1" ref="C28" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
+        <v>charsbckavmls</v>
+      </c>
+      <c r="D28" t="s">
+        <v>166</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Revisao models e modelsDTO, incluso testes unitarios
</commit_message>
<xml_diff>
--- a/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
+++ b/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c20d8aba5601db01/Documentos/00_DigitalHouse/06_BACKEND/00_trabalho_em_Grupo/dentalclinic/dentalclinic/src/test/java/br/com/dentalclinic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAEDB455-E3C3-4F57-B727-70AA9495471A}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0354B50B-E268-4C13-A946-B8244BAEEFF7}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE38068E-1540-4545-93C9-0DD6012C8E13}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="GeraEndereco" sheetId="3" r:id="rId1"/>
     <sheet name="Clinica" sheetId="4" r:id="rId2"/>
     <sheet name="Usuario" sheetId="5" r:id="rId3"/>
+    <sheet name="Dentista" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="222">
   <si>
     <t>logradouro</t>
   </si>
@@ -566,6 +567,165 @@
   </si>
   <si>
     <t>Administrador</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>cro</t>
+  </si>
+  <si>
+    <t>usuario</t>
+  </si>
+  <si>
+    <t>clinica</t>
+  </si>
+  <si>
+    <t>sobrenome</t>
+  </si>
+  <si>
+    <t>Carlu Dijkstra</t>
+  </si>
+  <si>
+    <t>Ferid Samara</t>
+  </si>
+  <si>
+    <t>Berlin Kumagai</t>
+  </si>
+  <si>
+    <t>Tito Nagy</t>
+  </si>
+  <si>
+    <t>Swaran Petrović</t>
+  </si>
+  <si>
+    <t>Xenokrates Lévêque</t>
+  </si>
+  <si>
+    <t>Sandeep Schuster</t>
+  </si>
+  <si>
+    <t>Naveen Mah</t>
+  </si>
+  <si>
+    <t>Ghayth Nifterick</t>
+  </si>
+  <si>
+    <t>Urbanus Whitney</t>
+  </si>
+  <si>
+    <t>Theophylaktos McCarthy</t>
+  </si>
+  <si>
+    <t>Abidemi D'Ambrosio</t>
+  </si>
+  <si>
+    <t>Sohail Genovese</t>
+  </si>
+  <si>
+    <t>Apoorva Láník</t>
+  </si>
+  <si>
+    <t>Safa Eliasson</t>
+  </si>
+  <si>
+    <t>Dudda Escamilla</t>
+  </si>
+  <si>
+    <t>Shyam Norup</t>
+  </si>
+  <si>
+    <t>Govinda Constantin</t>
+  </si>
+  <si>
+    <t>Péter Laninga</t>
+  </si>
+  <si>
+    <t>Matej Antonescu</t>
+  </si>
+  <si>
+    <t>Zevulun Greer</t>
+  </si>
+  <si>
+    <t>Elbert Coburn</t>
+  </si>
+  <si>
+    <t>Gilad Mehmedović</t>
+  </si>
+  <si>
+    <t>Branko Hansen</t>
+  </si>
+  <si>
+    <t>Carlu.Dijkstra@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Ferid.Samara@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Berlin.Kumagai@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Tito.Nagy@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Péter.Laninga@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Swaran.Petrović@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Xenokrates.Lévêque@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Sandeep.Schuster@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Naveen.Mah@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Ghayth.Nifterick@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Urbanus.Whitney@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Theophylaktos.McCarthy@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Abidemi.D'Ambrosio@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Sohail.Genovese@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Apoorva.Láník@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Safa.Eliasson@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Dudda.Escamilla@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Shyam.Norup@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Govinda.Constantin@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Matej.Antonescu@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Zevulun.Greer@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Elbert.Coburn@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Gilad.Mehmedović@clinica.com.br</t>
+  </si>
+  <si>
+    <t>Branko.Hansen@clinica.com.br</t>
   </si>
 </sst>
 </file>
@@ -656,13 +816,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1834,7 +1995,7 @@
   <dimension ref="C1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection activeCell="C2" sqref="C2:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,10 +2214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D6BEF-0063-487A-8FD9-30F4346C7EFC}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A28"/>
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,15 +2245,14 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f ca="1">B2&amp;";"&amp;C2&amp;";"&amp;D2</f>
-        <v>sgtbpsscharsv@pprovicer.com.br;sgtbpsscharsv;Administrador</v>
-      </c>
-      <c r="B2" t="str">
-        <f ca="1">C2&amp;"@pprovicer.com.br"</f>
-        <v>sgtbpsscharsv@pprovicer.com.br</v>
+        <v>Carlu.Dijkstra@clinica.com.br;eundmvcharsqg;Administrador</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>sgtbpsscharsv</v>
+        <v>eundmvcharsqg</v>
       </c>
       <c r="D2" t="s">
         <v>168</v>
@@ -2104,15 +2264,14 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A28" ca="1" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3</f>
-        <v>tyarrqbvm@pprovicer.com.br;tyarrqbvm;Dentista</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B28" ca="1" si="1">C3&amp;"@pprovicer.com.br"</f>
-        <v>tyarrqbvm@pprovicer.com.br</v>
+        <v>Ferid.Samara@clinica.com.br;gbadccharskgr;Dentista</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>tyarrqbvm</v>
+        <v>gbadccharskgr</v>
       </c>
       <c r="D3" t="s">
         <v>165</v>
@@ -2124,15 +2283,14 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>glqopbqschars@pprovicer.com.br;glqopbqschars;Recepcionista</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>glqopbqschars@pprovicer.com.br</v>
+        <v>Berlin.Kumagai@clinica.com.br;dulmfkqnu;Recepcionista</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>glqopbqschars</v>
+        <v>dulmfkqnu</v>
       </c>
       <c r="D4" t="s">
         <v>166</v>
@@ -2144,15 +2302,14 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>charsajntfhcs@pprovicer.com.br;charsajntfhcs;Paciente</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>charsajntfhcs@pprovicer.com.br</v>
+        <v>Tito.Nagy@clinica.com.br;jvehgcharsgrk;Paciente</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charsajntfhcs</v>
+        <v>jvehgcharsgrk</v>
       </c>
       <c r="D5" t="s">
         <v>167</v>
@@ -2164,15 +2321,14 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>umjccharsrjuo@pprovicer.com.br;umjccharsrjuo;Administrador</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>umjccharsrjuo@pprovicer.com.br</v>
+        <v>Péter.Laninga@clinica.com.br;fvbngjhjn;Administrador</v>
+      </c>
+      <c r="B6" t="s">
+        <v>202</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>umjccharsrjuo</v>
+        <v>fvbngjhjn</v>
       </c>
       <c r="D6" t="s">
         <v>168</v>
@@ -2184,15 +2340,14 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>ukiqjxhfe@pprovicer.com.br;ukiqjxhfe;Dentista</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>ukiqjxhfe@pprovicer.com.br</v>
+        <v>Swaran.Petrović@clinica.com.br;meovkoqbs;Dentista</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>ukiqjxhfe</v>
+        <v>meovkoqbs</v>
       </c>
       <c r="D7" t="s">
         <v>165</v>
@@ -2204,15 +2359,14 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>shmjtacharsur@pprovicer.com.br;shmjtacharsur;Recepcionista</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>shmjtacharsur@pprovicer.com.br</v>
+        <v>Xenokrates.Lévêque@clinica.com.br;jhcharsdrjkvi;Recepcionista</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>shmjtacharsur</v>
+        <v>jhcharsdrjkvi</v>
       </c>
       <c r="D8" t="s">
         <v>166</v>
@@ -2224,15 +2378,14 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>orcharslxboul@pprovicer.com.br;orcharslxboul;Paciente</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>orcharslxboul@pprovicer.com.br</v>
+        <v>Sandeep.Schuster@clinica.com.br;jjxphcucharso;Paciente</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>orcharslxboul</v>
+        <v>jjxphcucharso</v>
       </c>
       <c r="D9" t="s">
         <v>167</v>
@@ -2244,15 +2397,14 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>jvmxcharsmvle@pprovicer.com.br;jvmxcharsmvle;Administrador</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>jvmxcharsmvle@pprovicer.com.br</v>
+        <v>Naveen.Mah@clinica.com.br;ooaaenark;Administrador</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>jvmxcharsmvle</v>
+        <v>ooaaenark</v>
       </c>
       <c r="D10" t="s">
         <v>168</v>
@@ -2264,15 +2416,14 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>oaeratyoe@pprovicer.com.br;oaeratyoe;Dentista</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>oaeratyoe@pprovicer.com.br</v>
+        <v>Ghayth.Nifterick@clinica.com.br;fiegjuvjx;Dentista</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>oaeratyoe</v>
+        <v>fiegjuvjx</v>
       </c>
       <c r="D11" t="s">
         <v>165</v>
@@ -2284,15 +2435,14 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>charsuxyjvidb@pprovicer.com.br;charsuxyjvidb;Recepcionista</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>charsuxyjvidb@pprovicer.com.br</v>
+        <v>Urbanus.Whitney@clinica.com.br;bgvrievmf;Recepcionista</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charsuxyjvidb</v>
+        <v>bgvrievmf</v>
       </c>
       <c r="D12" t="s">
         <v>166</v>
@@ -2304,15 +2454,14 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>cjohjyumk@pprovicer.com.br;cjohjyumk;Paciente</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>cjohjyumk@pprovicer.com.br</v>
+        <v>Theophylaktos.McCarthy@clinica.com.br;xvinpcbsg;Paciente</v>
+      </c>
+      <c r="B13" t="s">
+        <v>209</v>
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>cjohjyumk</v>
+        <v>xvinpcbsg</v>
       </c>
       <c r="D13" t="s">
         <v>167</v>
@@ -2324,15 +2473,14 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>tespcxhcb@pprovicer.com.br;tespcxhcb;Administrador</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>tespcxhcb@pprovicer.com.br</v>
+        <v>Abidemi.D'Ambrosio@clinica.com.br;charsnxnpiitx;Administrador</v>
+      </c>
+      <c r="B14" t="s">
+        <v>210</v>
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>tespcxhcb</v>
+        <v>charsnxnpiitx</v>
       </c>
       <c r="D14" t="s">
         <v>168</v>
@@ -2344,15 +2492,14 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>rcharsvmuqtrf@pprovicer.com.br;rcharsvmuqtrf;Dentista</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>rcharsvmuqtrf@pprovicer.com.br</v>
+        <v>Sohail.Genovese@clinica.com.br;leekomjbr;Dentista</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>rcharsvmuqtrf</v>
+        <v>leekomjbr</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -2364,15 +2511,14 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>gegheenbchars@pprovicer.com.br;gegheenbchars;Recepcionista</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>gegheenbchars@pprovicer.com.br</v>
+        <v>Apoorva.Láník@clinica.com.br;rgkbhytco;Recepcionista</v>
+      </c>
+      <c r="B16" t="s">
+        <v>212</v>
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>gegheenbchars</v>
+        <v>rgkbhytco</v>
       </c>
       <c r="D16" t="s">
         <v>166</v>
@@ -2384,15 +2530,14 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>oagacharsxbjg@pprovicer.com.br;oagacharsxbjg;Paciente</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>oagacharsxbjg@pprovicer.com.br</v>
+        <v>Safa.Eliasson@clinica.com.br;sojfyiulc;Paciente</v>
+      </c>
+      <c r="B17" t="s">
+        <v>213</v>
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>oagacharsxbjg</v>
+        <v>sojfyiulc</v>
       </c>
       <c r="D17" t="s">
         <v>167</v>
@@ -2404,15 +2549,14 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>jibbvxgfl@pprovicer.com.br;jibbvxgfl;Administrador</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>jibbvxgfl@pprovicer.com.br</v>
+        <v>Dudda.Escamilla@clinica.com.br;lugycharsghrn;Administrador</v>
+      </c>
+      <c r="B18" t="s">
+        <v>214</v>
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>jibbvxgfl</v>
+        <v>lugycharsghrn</v>
       </c>
       <c r="D18" t="s">
         <v>168</v>
@@ -2424,15 +2568,14 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>charsstihrxlu@pprovicer.com.br;charsstihrxlu;Dentista</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>charsstihrxlu@pprovicer.com.br</v>
+        <v>Shyam.Norup@clinica.com.br;xftgqioso;Dentista</v>
+      </c>
+      <c r="B19" t="s">
+        <v>215</v>
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charsstihrxlu</v>
+        <v>xftgqioso</v>
       </c>
       <c r="D19" t="s">
         <v>165</v>
@@ -2444,15 +2587,14 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>kaphjyucharsb@pprovicer.com.br;kaphjyucharsb;Recepcionista</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>kaphjyucharsb@pprovicer.com.br</v>
+        <v>Govinda.Constantin@clinica.com.br;nryeqcprp;Recepcionista</v>
+      </c>
+      <c r="B20" t="s">
+        <v>216</v>
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>kaphjyucharsb</v>
+        <v>nryeqcprp</v>
       </c>
       <c r="D20" t="s">
         <v>166</v>
@@ -2464,15 +2606,14 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>puvbktlre@pprovicer.com.br;puvbktlre;Paciente</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>puvbktlre@pprovicer.com.br</v>
+        <v>Matej.Antonescu@clinica.com.br;dlmrcharsnqjc;Paciente</v>
+      </c>
+      <c r="B21" t="s">
+        <v>217</v>
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>puvbktlre</v>
+        <v>dlmrcharsnqjc</v>
       </c>
       <c r="D21" t="s">
         <v>167</v>
@@ -2484,15 +2625,14 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>uojjdgjvc@pprovicer.com.br;uojjdgjvc;Administrador</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>uojjdgjvc@pprovicer.com.br</v>
+        <v>Zevulun.Greer@clinica.com.br;rflisyanu;Administrador</v>
+      </c>
+      <c r="B22" t="s">
+        <v>218</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>uojjdgjvc</v>
+        <v>rflisyanu</v>
       </c>
       <c r="D22" t="s">
         <v>168</v>
@@ -2504,15 +2644,14 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>draohjsve@pprovicer.com.br;draohjsve;Dentista</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>draohjsve@pprovicer.com.br</v>
+        <v>Elbert.Coburn@clinica.com.br;eemjrmcue;Dentista</v>
+      </c>
+      <c r="B23" t="s">
+        <v>219</v>
       </c>
       <c r="C23" t="str" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>draohjsve</v>
+        <v>eemjrmcue</v>
       </c>
       <c r="D23" t="s">
         <v>165</v>
@@ -2524,15 +2663,14 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>qyfsrdoqchars@pprovicer.com.br;qyfsrdoqchars;Recepcionista</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>qyfsrdoqchars@pprovicer.com.br</v>
+        <v>Gilad.Mehmedović@clinica.com.br;gfqvbsixv;Recepcionista</v>
+      </c>
+      <c r="B24" t="s">
+        <v>220</v>
       </c>
       <c r="C24" t="str" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>qyfsrdoqchars</v>
+        <v>gfqvbsixv</v>
       </c>
       <c r="D24" t="s">
         <v>166</v>
@@ -2544,15 +2682,14 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>charscqnvinxt@pprovicer.com.br;charscqnvinxt;Paciente</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>charscqnvinxt@pprovicer.com.br</v>
+        <v>Branko.Hansen@clinica.com.br;qohuicharsitk;Paciente</v>
+      </c>
+      <c r="B25" t="s">
+        <v>221</v>
       </c>
       <c r="C25" t="str" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charscqnvinxt</v>
+        <v>qohuicharsitk</v>
       </c>
       <c r="D25" t="s">
         <v>167</v>
@@ -2562,61 +2699,754 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>fecharsnojgnchars@pprovicer.com.br;fecharsnojgnchars;Administrador</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>fecharsnojgnchars@pprovicer.com.br</v>
-      </c>
-      <c r="C26" t="str" cm="1">
-        <f t="array" aca="1" ref="C26" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>fecharsnojgnchars</v>
-      </c>
-      <c r="D26" t="s">
-        <v>168</v>
-      </c>
       <c r="G26" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>lgevkrkfm@pprovicer.com.br;lgevkrkfm;Dentista</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>lgevkrkfm@pprovicer.com.br</v>
-      </c>
-      <c r="C27" t="str" cm="1">
-        <f t="array" aca="1" ref="C27" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>lgevkrkfm</v>
-      </c>
-      <c r="D27" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>charsbckavmls@pprovicer.com.br;charsbckavmls;Recepcionista</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>charsbckavmls@pprovicer.com.br</v>
-      </c>
-      <c r="C28" t="str" cm="1">
-        <f t="array" aca="1" ref="C28" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charsbckavmls</v>
-      </c>
-      <c r="D28" t="s">
-        <v>166</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE08DE9A-8FF7-4B04-AEFD-6718A0B2BDDD}">
+  <dimension ref="A1:J25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B2" t="str">
+        <f>LEFT(A2,FIND(" ",A2,1)-1)</f>
+        <v>Carlu</v>
+      </c>
+      <c r="C2" t="str">
+        <f>RIGHT(A2,LEN(A2)-FIND(" ",A2,1))</f>
+        <v>Dijkstra</v>
+      </c>
+      <c r="D2" t="str" cm="1">
+        <f t="array" aca="1" ref="D2" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>675634</v>
+      </c>
+      <c r="F2" t="str">
+        <f>B2&amp;"."&amp;C2&amp;"@clinica.com.br"</f>
+        <v>Carlu.Dijkstra@clinica.com.br</v>
+      </c>
+      <c r="G2" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <f ca="1">B2&amp;";"&amp;C2&amp;";"&amp;D2&amp;";"&amp;F2&amp;";"&amp;G2</f>
+        <v>Carlu;Dijkstra;675634;Carlu.Dijkstra@clinica.com.br;Consultorio Sorisso Feliz</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B25" si="0">LEFT(A3,FIND(" ",A3,1)-1)</f>
+        <v>Ferid</v>
+      </c>
+      <c r="C3" t="str">
+        <f>RIGHT(A3,LEN(A3)-FIND(" ",A3,1))</f>
+        <v>Samara</v>
+      </c>
+      <c r="D3" t="str" cm="1">
+        <f t="array" aca="1" ref="D3" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>478617</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F25" si="1">B3&amp;"."&amp;C3&amp;"@clinica.com.br"</f>
+        <v>Ferid.Samara@clinica.com.br</v>
+      </c>
+      <c r="G3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="6">
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J25" ca="1" si="2">B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;F3&amp;";"&amp;G3</f>
+        <v>Ferid;Samara;478617;Ferid.Samara@clinica.com.br;Clinica Joseph Climber</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Berlin</v>
+      </c>
+      <c r="C4" t="str">
+        <f>RIGHT(A4,LEN(A4)-FIND(" ",A4,1))</f>
+        <v>Kumagai</v>
+      </c>
+      <c r="D4" t="str" cm="1">
+        <f t="array" aca="1" ref="D4" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>756772</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>Berlin.Kumagai@clinica.com.br</v>
+      </c>
+      <c r="G4" t="s">
+        <v>122</v>
+      </c>
+      <c r="I4" s="6">
+        <v>2</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Berlin;Kumagai;756772;Berlin.Kumagai@clinica.com.br;Consultorio Dentes Brilhantes</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Tito</v>
+      </c>
+      <c r="C5" t="str">
+        <f>RIGHT(A5,LEN(A5)-FIND(" ",A5,1))</f>
+        <v>Nagy</v>
+      </c>
+      <c r="D5" t="str" cm="1">
+        <f t="array" aca="1" ref="D5" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>999674</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>Tito.Nagy@clinica.com.br</v>
+      </c>
+      <c r="G5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="6">
+        <v>3</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Tito;Nagy;999674;Tito.Nagy@clinica.com.br;Clinica do Manuel</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Péter</v>
+      </c>
+      <c r="C6" t="str">
+        <f>RIGHT(A6,LEN(A6)-FIND(" ",A6,1))</f>
+        <v>Laninga</v>
+      </c>
+      <c r="D6" t="str" cm="1">
+        <f t="array" aca="1" ref="D6" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>985366</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>Péter.Laninga@clinica.com.br</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Péter;Laninga;985366;Péter.Laninga@clinica.com.br;Consultorio Sorridente</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Swaran</v>
+      </c>
+      <c r="C7" t="str">
+        <f>RIGHT(A7,LEN(A7)-FIND(" ",A7,1))</f>
+        <v>Petrović</v>
+      </c>
+      <c r="D7" t="str" cm="1">
+        <f t="array" aca="1" ref="D7" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>763443</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>Swaran.Petrović@clinica.com.br</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="6">
+        <v>5</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Swaran;Petrović;763443;Swaran.Petrović@clinica.com.br;Clinica da Esquina</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Xenokrates</v>
+      </c>
+      <c r="C8" t="str">
+        <f>RIGHT(A8,LEN(A8)-FIND(" ",A8,1))</f>
+        <v>Lévêque</v>
+      </c>
+      <c r="D8" t="str" cm="1">
+        <f t="array" aca="1" ref="D8" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>366489</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>Xenokrates.Lévêque@clinica.com.br</v>
+      </c>
+      <c r="G8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="6">
+        <v>6</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Xenokrates;Lévêque;366489;Xenokrates.Lévêque@clinica.com.br;Consultorio Sorriso Maroto</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Sandeep</v>
+      </c>
+      <c r="C9" t="str">
+        <f>RIGHT(A9,LEN(A9)-FIND(" ",A9,1))</f>
+        <v>Schuster</v>
+      </c>
+      <c r="D9" t="str" cm="1">
+        <f t="array" aca="1" ref="D9" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>393535</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>Sandeep.Schuster@clinica.com.br</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="6">
+        <v>7</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Sandeep;Schuster;393535;Sandeep.Schuster@clinica.com.br;Clinica Marota</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Naveen</v>
+      </c>
+      <c r="C10" t="str">
+        <f>RIGHT(A10,LEN(A10)-FIND(" ",A10,1))</f>
+        <v>Mah</v>
+      </c>
+      <c r="D10" t="str" cm="1">
+        <f t="array" aca="1" ref="D10" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>523729</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>Naveen.Mah@clinica.com.br</v>
+      </c>
+      <c r="G10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="6">
+        <v>8</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Naveen;Mah;523729;Naveen.Mah@clinica.com.br;Consultorio Sorriso Branquinho</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Ghayth</v>
+      </c>
+      <c r="C11" t="str">
+        <f>RIGHT(A11,LEN(A11)-FIND(" ",A11,1))</f>
+        <v>Nifterick</v>
+      </c>
+      <c r="D11" t="str" cm="1">
+        <f t="array" aca="1" ref="D11" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>680508</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>Ghayth.Nifterick@clinica.com.br</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="6">
+        <v>9</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Ghayth;Nifterick;680508;Ghayth.Nifterick@clinica.com.br;Clinica Legal</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>183</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Urbanus</v>
+      </c>
+      <c r="C12" t="str">
+        <f>RIGHT(A12,LEN(A12)-FIND(" ",A12,1))</f>
+        <v>Whitney</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" aca="1" ref="D12" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>027292</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>Urbanus.Whitney@clinica.com.br</v>
+      </c>
+      <c r="G12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="6"/>
+      <c r="J12" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Urbanus;Whitney;027292;Urbanus.Whitney@clinica.com.br;Consultorio Dentes Brilhantes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Theophylaktos</v>
+      </c>
+      <c r="C13" t="str">
+        <f>RIGHT(A13,LEN(A13)-FIND(" ",A13,1))</f>
+        <v>McCarthy</v>
+      </c>
+      <c r="D13" t="str" cm="1">
+        <f t="array" aca="1" ref="D13" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>084181</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>Theophylaktos.McCarthy@clinica.com.br</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Theophylaktos;McCarthy;084181;Theophylaktos.McCarthy@clinica.com.br;Clinica Da Avenida</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>185</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Abidemi</v>
+      </c>
+      <c r="C14" t="str">
+        <f>RIGHT(A14,LEN(A14)-FIND(" ",A14,1))</f>
+        <v>D'Ambrosio</v>
+      </c>
+      <c r="D14" t="str" cm="1">
+        <f t="array" aca="1" ref="D14" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>879341</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>Abidemi.D'Ambrosio@clinica.com.br</v>
+      </c>
+      <c r="G14" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Abidemi;D'Ambrosio;879341;Abidemi.D'Ambrosio@clinica.com.br;Consultorio Sorriso Contagiante</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Sohail</v>
+      </c>
+      <c r="C15" t="str">
+        <f>RIGHT(A15,LEN(A15)-FIND(" ",A15,1))</f>
+        <v>Genovese</v>
+      </c>
+      <c r="D15" t="str" cm="1">
+        <f t="array" aca="1" ref="D15" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>363053</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>Sohail.Genovese@clinica.com.br</v>
+      </c>
+      <c r="G15" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Sohail;Genovese;363053;Sohail.Genovese@clinica.com.br;Clinica Popular</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Apoorva</v>
+      </c>
+      <c r="C16" t="str">
+        <f>RIGHT(A16,LEN(A16)-FIND(" ",A16,1))</f>
+        <v>Láník</v>
+      </c>
+      <c r="D16" t="str" cm="1">
+        <f t="array" aca="1" ref="D16" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>622949</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>Apoorva.Láník@clinica.com.br</v>
+      </c>
+      <c r="G16" t="s">
+        <v>133</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Apoorva;Láník;622949;Apoorva.Láník@clinica.com.br;Consultorio Saudente</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Safa</v>
+      </c>
+      <c r="C17" t="str">
+        <f>RIGHT(A17,LEN(A17)-FIND(" ",A17,1))</f>
+        <v>Eliasson</v>
+      </c>
+      <c r="D17" t="str" cm="1">
+        <f t="array" aca="1" ref="D17" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>155593</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>Safa.Eliasson@clinica.com.br</v>
+      </c>
+      <c r="G17" t="s">
+        <v>135</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Safa;Eliasson;155593;Safa.Eliasson@clinica.com.br;Clinica Mega Popular</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Dudda</v>
+      </c>
+      <c r="C18" t="str">
+        <f>RIGHT(A18,LEN(A18)-FIND(" ",A18,1))</f>
+        <v>Escamilla</v>
+      </c>
+      <c r="D18" t="str" cm="1">
+        <f t="array" aca="1" ref="D18" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>145003</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>Dudda.Escamilla@clinica.com.br</v>
+      </c>
+      <c r="G18" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Dudda;Escamilla;145003;Dudda.Escamilla@clinica.com.br;Consultorio Sorisso Feliz</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Shyam</v>
+      </c>
+      <c r="C19" t="str">
+        <f>RIGHT(A19,LEN(A19)-FIND(" ",A19,1))</f>
+        <v>Norup</v>
+      </c>
+      <c r="D19" t="str" cm="1">
+        <f t="array" aca="1" ref="D19" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>696430</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>Shyam.Norup@clinica.com.br</v>
+      </c>
+      <c r="G19" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Shyam;Norup;696430;Shyam.Norup@clinica.com.br;Clinica Joseph Climber</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Govinda</v>
+      </c>
+      <c r="C20" t="str">
+        <f>RIGHT(A20,LEN(A20)-FIND(" ",A20,1))</f>
+        <v>Constantin</v>
+      </c>
+      <c r="D20" t="str" cm="1">
+        <f t="array" aca="1" ref="D20" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>212291</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>Govinda.Constantin@clinica.com.br</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Govinda;Constantin;212291;Govinda.Constantin@clinica.com.br;Consultorio Dentes Brilhantes</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Matej</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" ref="C21:C25" si="3">RIGHT(A21,LEN(A21)-FIND(" ",A21,1))</f>
+        <v>Antonescu</v>
+      </c>
+      <c r="D21" t="str" cm="1">
+        <f t="array" aca="1" ref="D21" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>860443</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>Matej.Antonescu@clinica.com.br</v>
+      </c>
+      <c r="G21" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Matej;Antonescu;860443;Matej.Antonescu@clinica.com.br;Clinica do Manuel</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>194</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Zevulun</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="3"/>
+        <v>Greer</v>
+      </c>
+      <c r="D22" t="str" cm="1">
+        <f t="array" aca="1" ref="D22" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>620938</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="1"/>
+        <v>Zevulun.Greer@clinica.com.br</v>
+      </c>
+      <c r="G22" t="s">
+        <v>124</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Zevulun;Greer;620938;Zevulun.Greer@clinica.com.br;Consultorio Sorridente</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Elbert</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="3"/>
+        <v>Coburn</v>
+      </c>
+      <c r="D23" t="str" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>756846</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="1"/>
+        <v>Elbert.Coburn@clinica.com.br</v>
+      </c>
+      <c r="G23" t="s">
+        <v>125</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Elbert;Coburn;756846;Elbert.Coburn@clinica.com.br;Clinica da Esquina</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Gilad</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="3"/>
+        <v>Mehmedović</v>
+      </c>
+      <c r="D24" t="str" cm="1">
+        <f t="array" aca="1" ref="D24" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>526330</v>
+      </c>
+      <c r="F24" t="str">
+        <f t="shared" si="1"/>
+        <v>Gilad.Mehmedović@clinica.com.br</v>
+      </c>
+      <c r="G24" t="s">
+        <v>126</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Gilad;Mehmedović;526330;Gilad.Mehmedović@clinica.com.br;Consultorio Sorriso Maroto</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>197</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Branko</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="3"/>
+        <v>Hansen</v>
+      </c>
+      <c r="D25" t="str" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
+        <v>923147</v>
+      </c>
+      <c r="F25" t="str">
+        <f t="shared" si="1"/>
+        <v>Branko.Hansen@clinica.com.br</v>
+      </c>
+      <c r="G25" t="s">
+        <v>127</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>Branko;Hansen;923147;Branko.Hansen@clinica.com.br;Clinica Marota</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Atualizacao dos testes unitarios
</commit_message>
<xml_diff>
--- a/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
+++ b/dentalclinic/src/test/java/br/com/dentalclinic/PlanilhaGeradoraDadosTestes.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c20d8aba5601db01/Documentos/00_DigitalHouse/06_BACKEND/00_trabalho_em_Grupo/dentalclinic/dentalclinic/src/test/java/br/com/dentalclinic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0354B50B-E268-4C13-A946-B8244BAEEFF7}"/>
+  <xr:revisionPtr revIDLastSave="286" documentId="8_{1CA44F3D-27D1-4F99-B8EA-8FA4536F3FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF723454-32BB-4B65-A19E-6301D2C83E8B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EE38068E-1540-4545-93C9-0DD6012C8E13}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{EE38068E-1540-4545-93C9-0DD6012C8E13}"/>
   </bookViews>
   <sheets>
     <sheet name="GeraEndereco" sheetId="3" r:id="rId1"/>
     <sheet name="Clinica" sheetId="4" r:id="rId2"/>
     <sheet name="Usuario" sheetId="5" r:id="rId3"/>
     <sheet name="Dentista" sheetId="6" r:id="rId4"/>
+    <sheet name="Paciente" sheetId="7" r:id="rId5"/>
+    <sheet name="Consulta" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="268">
   <si>
     <t>logradouro</t>
   </si>
@@ -726,6 +728,144 @@
   </si>
   <si>
     <t>Branko.Hansen@clinica.com.br</t>
+  </si>
+  <si>
+    <t>cpf</t>
+  </si>
+  <si>
+    <t>telefone</t>
+  </si>
+  <si>
+    <t>endereco</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Pedro</t>
+  </si>
+  <si>
+    <t>Fabio</t>
+  </si>
+  <si>
+    <t>Neres</t>
+  </si>
+  <si>
+    <t>Sankler</t>
+  </si>
+  <si>
+    <t>Bergman</t>
+  </si>
+  <si>
+    <t>Tiago</t>
+  </si>
+  <si>
+    <t>Pereira</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Furukawa</t>
+  </si>
+  <si>
+    <t>Joao</t>
+  </si>
+  <si>
+    <t>Santos</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Gasolina</t>
+  </si>
+  <si>
+    <t>Joana</t>
+  </si>
+  <si>
+    <t>da Silva</t>
+  </si>
+  <si>
+    <t>Jacinto</t>
+  </si>
+  <si>
+    <t>Pinto</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
+    <t>Artur</t>
+  </si>
+  <si>
+    <t>Norberto</t>
+  </si>
+  <si>
+    <t>Jurema</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Bernardo</t>
+  </si>
+  <si>
+    <t>Cornwell</t>
+  </si>
+  <si>
+    <t>Josefina</t>
+  </si>
+  <si>
+    <t>Mata</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Marta</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>ANO</t>
+  </si>
+  <si>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>DIA</t>
+  </si>
+  <si>
+    <t>hora</t>
+  </si>
+  <si>
+    <t>minuto</t>
+  </si>
+  <si>
+    <t>banguela</t>
+  </si>
+  <si>
+    <t>dentadura</t>
+  </si>
+  <si>
+    <t>dor de dente</t>
+  </si>
+  <si>
+    <t>confirmada</t>
+  </si>
+  <si>
+    <t>encerrada</t>
+  </si>
+  <si>
+    <t>pendente</t>
+  </si>
+  <si>
+    <t>cancelada</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1281,7 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="E17" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2216,7 +2356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F7D6BEF-0063-487A-8FD9-30F4346C7EFC}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
@@ -2245,14 +2385,14 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f ca="1">B2&amp;";"&amp;C2&amp;";"&amp;D2</f>
-        <v>Carlu.Dijkstra@clinica.com.br;eundmvcharsqg;Administrador</v>
+        <v>Carlu.Dijkstra@clinica.com.br;sbuvunkns;Administrador</v>
       </c>
       <c r="B2" t="s">
         <v>198</v>
       </c>
       <c r="C2" t="str" cm="1">
         <f t="array" aca="1" ref="C2" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>eundmvcharsqg</v>
+        <v>sbuvunkns</v>
       </c>
       <c r="D2" t="s">
         <v>168</v>
@@ -2263,15 +2403,15 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A28" ca="1" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3</f>
-        <v>Ferid.Samara@clinica.com.br;gbadccharskgr;Dentista</v>
+        <f t="shared" ref="A3:A25" ca="1" si="0">B3&amp;";"&amp;C3&amp;";"&amp;D3</f>
+        <v>Ferid.Samara@clinica.com.br;jxsidlmfg;Dentista</v>
       </c>
       <c r="B3" t="s">
         <v>199</v>
       </c>
       <c r="C3" t="str" cm="1">
         <f t="array" aca="1" ref="C3" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>gbadccharskgr</v>
+        <v>jxsidlmfg</v>
       </c>
       <c r="D3" t="s">
         <v>165</v>
@@ -2283,14 +2423,14 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Berlin.Kumagai@clinica.com.br;dulmfkqnu;Recepcionista</v>
+        <v>Berlin.Kumagai@clinica.com.br;ptsfryjjx;Recepcionista</v>
       </c>
       <c r="B4" t="s">
         <v>200</v>
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>dulmfkqnu</v>
+        <v>ptsfryjjx</v>
       </c>
       <c r="D4" t="s">
         <v>166</v>
@@ -2302,14 +2442,14 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tito.Nagy@clinica.com.br;jvehgcharsgrk;Paciente</v>
+        <v>Tito.Nagy@clinica.com.br;lacvyljgy;Paciente</v>
       </c>
       <c r="B5" t="s">
         <v>201</v>
       </c>
       <c r="C5" t="str" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>jvehgcharsgrk</v>
+        <v>lacvyljgy</v>
       </c>
       <c r="D5" t="s">
         <v>167</v>
@@ -2321,14 +2461,14 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Péter.Laninga@clinica.com.br;fvbngjhjn;Administrador</v>
+        <v>Péter.Laninga@clinica.com.br;charsencgcharscae;Administrador</v>
       </c>
       <c r="B6" t="s">
         <v>202</v>
       </c>
       <c r="C6" t="str" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>fvbngjhjn</v>
+        <v>charsencgcharscae</v>
       </c>
       <c r="D6" t="s">
         <v>168</v>
@@ -2340,14 +2480,14 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Swaran.Petrović@clinica.com.br;meovkoqbs;Dentista</v>
+        <v>Swaran.Petrović@clinica.com.br;lqvuvkcharsgh;Dentista</v>
       </c>
       <c r="B7" t="s">
         <v>203</v>
       </c>
       <c r="C7" t="str" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>meovkoqbs</v>
+        <v>lqvuvkcharsgh</v>
       </c>
       <c r="D7" t="s">
         <v>165</v>
@@ -2359,14 +2499,14 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Xenokrates.Lévêque@clinica.com.br;jhcharsdrjkvi;Recepcionista</v>
+        <v>Xenokrates.Lévêque@clinica.com.br;prbcharstpepx;Recepcionista</v>
       </c>
       <c r="B8" t="s">
         <v>204</v>
       </c>
       <c r="C8" t="str" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>jhcharsdrjkvi</v>
+        <v>prbcharstpepx</v>
       </c>
       <c r="D8" t="s">
         <v>166</v>
@@ -2378,14 +2518,14 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sandeep.Schuster@clinica.com.br;jjxphcucharso;Paciente</v>
+        <v>Sandeep.Schuster@clinica.com.br;ykjixkjbe;Paciente</v>
       </c>
       <c r="B9" t="s">
         <v>205</v>
       </c>
       <c r="C9" t="str" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>jjxphcucharso</v>
+        <v>ykjixkjbe</v>
       </c>
       <c r="D9" t="s">
         <v>167</v>
@@ -2397,14 +2537,14 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Naveen.Mah@clinica.com.br;ooaaenark;Administrador</v>
+        <v>Naveen.Mah@clinica.com.br;fucbiyiae;Administrador</v>
       </c>
       <c r="B10" t="s">
         <v>206</v>
       </c>
       <c r="C10" t="str" cm="1">
         <f t="array" aca="1" ref="C10" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>ooaaenark</v>
+        <v>fucbiyiae</v>
       </c>
       <c r="D10" t="s">
         <v>168</v>
@@ -2416,14 +2556,14 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Ghayth.Nifterick@clinica.com.br;fiegjuvjx;Dentista</v>
+        <v>Ghayth.Nifterick@clinica.com.br;khkbttqsq;Dentista</v>
       </c>
       <c r="B11" t="s">
         <v>207</v>
       </c>
       <c r="C11" t="str" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>fiegjuvjx</v>
+        <v>khkbttqsq</v>
       </c>
       <c r="D11" t="s">
         <v>165</v>
@@ -2435,14 +2575,14 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Urbanus.Whitney@clinica.com.br;bgvrievmf;Recepcionista</v>
+        <v>Urbanus.Whitney@clinica.com.br;jqhjscharsmds;Recepcionista</v>
       </c>
       <c r="B12" t="s">
         <v>208</v>
       </c>
       <c r="C12" t="str" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>bgvrievmf</v>
+        <v>jqhjscharsmds</v>
       </c>
       <c r="D12" t="s">
         <v>166</v>
@@ -2454,14 +2594,14 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Theophylaktos.McCarthy@clinica.com.br;xvinpcbsg;Paciente</v>
+        <v>Theophylaktos.McCarthy@clinica.com.br;hrydrupss;Paciente</v>
       </c>
       <c r="B13" t="s">
         <v>209</v>
       </c>
       <c r="C13" t="str" cm="1">
         <f t="array" aca="1" ref="C13" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>xvinpcbsg</v>
+        <v>hrydrupss</v>
       </c>
       <c r="D13" t="s">
         <v>167</v>
@@ -2473,14 +2613,14 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Abidemi.D'Ambrosio@clinica.com.br;charsnxnpiitx;Administrador</v>
+        <v>Abidemi.D'Ambrosio@clinica.com.br;vbmuodqhm;Administrador</v>
       </c>
       <c r="B14" t="s">
         <v>210</v>
       </c>
       <c r="C14" t="str" cm="1">
         <f t="array" aca="1" ref="C14" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>charsnxnpiitx</v>
+        <v>vbmuodqhm</v>
       </c>
       <c r="D14" t="s">
         <v>168</v>
@@ -2492,14 +2632,14 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Sohail.Genovese@clinica.com.br;leekomjbr;Dentista</v>
+        <v>Sohail.Genovese@clinica.com.br;bqluocyxy;Dentista</v>
       </c>
       <c r="B15" t="s">
         <v>211</v>
       </c>
       <c r="C15" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>leekomjbr</v>
+        <v>bqluocyxy</v>
       </c>
       <c r="D15" t="s">
         <v>165</v>
@@ -2511,14 +2651,14 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Apoorva.Láník@clinica.com.br;rgkbhytco;Recepcionista</v>
+        <v>Apoorva.Láník@clinica.com.br;reroqyfmd;Recepcionista</v>
       </c>
       <c r="B16" t="s">
         <v>212</v>
       </c>
       <c r="C16" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>rgkbhytco</v>
+        <v>reroqyfmd</v>
       </c>
       <c r="D16" t="s">
         <v>166</v>
@@ -2530,14 +2670,14 @@
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Safa.Eliasson@clinica.com.br;sojfyiulc;Paciente</v>
+        <v>Safa.Eliasson@clinica.com.br;lohlkcmyv;Paciente</v>
       </c>
       <c r="B17" t="s">
         <v>213</v>
       </c>
       <c r="C17" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>sojfyiulc</v>
+        <v>lohlkcmyv</v>
       </c>
       <c r="D17" t="s">
         <v>167</v>
@@ -2549,14 +2689,14 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Dudda.Escamilla@clinica.com.br;lugycharsghrn;Administrador</v>
+        <v>Dudda.Escamilla@clinica.com.br;qvccqbdtd;Administrador</v>
       </c>
       <c r="B18" t="s">
         <v>214</v>
       </c>
       <c r="C18" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>lugycharsghrn</v>
+        <v>qvccqbdtd</v>
       </c>
       <c r="D18" t="s">
         <v>168</v>
@@ -2568,14 +2708,14 @@
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Shyam.Norup@clinica.com.br;xftgqioso;Dentista</v>
+        <v>Shyam.Norup@clinica.com.br;ejokixrtx;Dentista</v>
       </c>
       <c r="B19" t="s">
         <v>215</v>
       </c>
       <c r="C19" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>xftgqioso</v>
+        <v>ejokixrtx</v>
       </c>
       <c r="D19" t="s">
         <v>165</v>
@@ -2587,14 +2727,14 @@
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Govinda.Constantin@clinica.com.br;nryeqcprp;Recepcionista</v>
+        <v>Govinda.Constantin@clinica.com.br;myvgcharsxjek;Recepcionista</v>
       </c>
       <c r="B20" t="s">
         <v>216</v>
       </c>
       <c r="C20" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>nryeqcprp</v>
+        <v>myvgcharsxjek</v>
       </c>
       <c r="D20" t="s">
         <v>166</v>
@@ -2606,14 +2746,14 @@
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Matej.Antonescu@clinica.com.br;dlmrcharsnqjc;Paciente</v>
+        <v>Matej.Antonescu@clinica.com.br;ojsdsxjkl;Paciente</v>
       </c>
       <c r="B21" t="s">
         <v>217</v>
       </c>
       <c r="C21" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>dlmrcharsnqjc</v>
+        <v>ojsdsxjkl</v>
       </c>
       <c r="D21" t="s">
         <v>167</v>
@@ -2625,14 +2765,14 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Zevulun.Greer@clinica.com.br;rflisyanu;Administrador</v>
+        <v>Zevulun.Greer@clinica.com.br;takhnbbef;Administrador</v>
       </c>
       <c r="B22" t="s">
         <v>218</v>
       </c>
       <c r="C22" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>rflisyanu</v>
+        <v>takhnbbef</v>
       </c>
       <c r="D22" t="s">
         <v>168</v>
@@ -2644,14 +2784,14 @@
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Elbert.Coburn@clinica.com.br;eemjrmcue;Dentista</v>
+        <v>Elbert.Coburn@clinica.com.br;yegbsbdqr;Dentista</v>
       </c>
       <c r="B23" t="s">
         <v>219</v>
       </c>
       <c r="C23" t="str" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>eemjrmcue</v>
+        <v>yegbsbdqr</v>
       </c>
       <c r="D23" t="s">
         <v>165</v>
@@ -2663,14 +2803,14 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Gilad.Mehmedović@clinica.com.br;gfqvbsixv;Recepcionista</v>
+        <v>Gilad.Mehmedović@clinica.com.br;vkmrebcbq;Recepcionista</v>
       </c>
       <c r="B24" t="s">
         <v>220</v>
       </c>
       <c r="C24" t="str" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>gfqvbsixv</v>
+        <v>vkmrebcbq</v>
       </c>
       <c r="D24" t="s">
         <v>166</v>
@@ -2682,14 +2822,14 @@
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Branko.Hansen@clinica.com.br;qohuicharsitk;Paciente</v>
+        <v>Branko.Hansen@clinica.com.br;oanjskood;Paciente</v>
       </c>
       <c r="B25" t="s">
         <v>221</v>
       </c>
       <c r="C25" t="str" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_xlfn.TEXTJOIN("",1,INDEX($G$1:$G$26,_xlfn.RANDARRAY(9,1,1,25,TRUE)))</f>
-        <v>qohuicharsitk</v>
+        <v>oanjskood</v>
       </c>
       <c r="D25" t="s">
         <v>167</v>
@@ -2713,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE08DE9A-8FF7-4B04-AEFD-6718A0B2BDDD}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F25"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2724,6 +2864,7 @@
     <col min="6" max="6" width="38" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="90.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2752,12 +2893,12 @@
         <v>Carlu</v>
       </c>
       <c r="C2" t="str">
-        <f>RIGHT(A2,LEN(A2)-FIND(" ",A2,1))</f>
+        <f t="shared" ref="C2:C20" si="0">RIGHT(A2,LEN(A2)-FIND(" ",A2,1))</f>
         <v>Dijkstra</v>
       </c>
       <c r="D2" t="str" cm="1">
         <f t="array" aca="1" ref="D2" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>675634</v>
+        <v>218981</v>
       </c>
       <c r="F2" t="str">
         <f>B2&amp;"."&amp;C2&amp;"@clinica.com.br"</f>
@@ -2771,7 +2912,7 @@
       </c>
       <c r="J2" t="str">
         <f ca="1">B2&amp;";"&amp;C2&amp;";"&amp;D2&amp;";"&amp;F2&amp;";"&amp;G2</f>
-        <v>Carlu;Dijkstra;675634;Carlu.Dijkstra@clinica.com.br;Consultorio Sorisso Feliz</v>
+        <v>Carlu;Dijkstra;218981;Carlu.Dijkstra@clinica.com.br;Consultorio Sorisso Feliz</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2779,19 +2920,19 @@
         <v>175</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B25" si="0">LEFT(A3,FIND(" ",A3,1)-1)</f>
+        <f t="shared" ref="B3:B25" si="1">LEFT(A3,FIND(" ",A3,1)-1)</f>
         <v>Ferid</v>
       </c>
       <c r="C3" t="str">
-        <f>RIGHT(A3,LEN(A3)-FIND(" ",A3,1))</f>
+        <f t="shared" si="0"/>
         <v>Samara</v>
       </c>
       <c r="D3" t="str" cm="1">
         <f t="array" aca="1" ref="D3" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>478617</v>
+        <v>646570</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F25" si="1">B3&amp;"."&amp;C3&amp;"@clinica.com.br"</f>
+        <f t="shared" ref="F3:F25" si="2">B3&amp;"."&amp;C3&amp;"@clinica.com.br"</f>
         <v>Ferid.Samara@clinica.com.br</v>
       </c>
       <c r="G3" t="s">
@@ -2801,8 +2942,8 @@
         <v>1</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J25" ca="1" si="2">B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;F3&amp;";"&amp;G3</f>
-        <v>Ferid;Samara;478617;Ferid.Samara@clinica.com.br;Clinica Joseph Climber</v>
+        <f t="shared" ref="J3:J25" ca="1" si="3">B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;F3&amp;";"&amp;G3</f>
+        <v>Ferid;Samara;646570;Ferid.Samara@clinica.com.br;Clinica Joseph Climber</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2810,19 +2951,19 @@
         <v>176</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Berlin</v>
       </c>
       <c r="C4" t="str">
-        <f>RIGHT(A4,LEN(A4)-FIND(" ",A4,1))</f>
+        <f t="shared" si="0"/>
         <v>Kumagai</v>
       </c>
       <c r="D4" t="str" cm="1">
         <f t="array" aca="1" ref="D4" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>756772</v>
+        <v>477799</v>
       </c>
       <c r="F4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Berlin.Kumagai@clinica.com.br</v>
       </c>
       <c r="G4" t="s">
@@ -2832,8 +2973,8 @@
         <v>2</v>
       </c>
       <c r="J4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Berlin;Kumagai;756772;Berlin.Kumagai@clinica.com.br;Consultorio Dentes Brilhantes</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Berlin;Kumagai;477799;Berlin.Kumagai@clinica.com.br;Consultorio Dentes Brilhantes</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2841,19 +2982,19 @@
         <v>177</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Tito</v>
       </c>
       <c r="C5" t="str">
-        <f>RIGHT(A5,LEN(A5)-FIND(" ",A5,1))</f>
+        <f t="shared" si="0"/>
         <v>Nagy</v>
       </c>
       <c r="D5" t="str" cm="1">
         <f t="array" aca="1" ref="D5" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>999674</v>
+        <v>174955</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Tito.Nagy@clinica.com.br</v>
       </c>
       <c r="G5" t="s">
@@ -2863,8 +3004,8 @@
         <v>3</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Tito;Nagy;999674;Tito.Nagy@clinica.com.br;Clinica do Manuel</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Tito;Nagy;174955;Tito.Nagy@clinica.com.br;Clinica do Manuel</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2872,19 +3013,19 @@
         <v>192</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Péter</v>
       </c>
       <c r="C6" t="str">
-        <f>RIGHT(A6,LEN(A6)-FIND(" ",A6,1))</f>
+        <f t="shared" si="0"/>
         <v>Laninga</v>
       </c>
       <c r="D6" t="str" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>985366</v>
+        <v>420184</v>
       </c>
       <c r="F6" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Péter.Laninga@clinica.com.br</v>
       </c>
       <c r="G6" t="s">
@@ -2894,8 +3035,8 @@
         <v>4</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Péter;Laninga;985366;Péter.Laninga@clinica.com.br;Consultorio Sorridente</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Péter;Laninga;420184;Péter.Laninga@clinica.com.br;Consultorio Sorridente</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2903,19 +3044,19 @@
         <v>178</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Swaran</v>
       </c>
       <c r="C7" t="str">
-        <f>RIGHT(A7,LEN(A7)-FIND(" ",A7,1))</f>
+        <f t="shared" si="0"/>
         <v>Petrović</v>
       </c>
       <c r="D7" t="str" cm="1">
         <f t="array" aca="1" ref="D7" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>763443</v>
+        <v>630514</v>
       </c>
       <c r="F7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Swaran.Petrović@clinica.com.br</v>
       </c>
       <c r="G7" t="s">
@@ -2925,8 +3066,8 @@
         <v>5</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Swaran;Petrović;763443;Swaran.Petrović@clinica.com.br;Clinica da Esquina</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Swaran;Petrović;630514;Swaran.Petrović@clinica.com.br;Clinica da Esquina</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2934,19 +3075,19 @@
         <v>179</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Xenokrates</v>
       </c>
       <c r="C8" t="str">
-        <f>RIGHT(A8,LEN(A8)-FIND(" ",A8,1))</f>
+        <f t="shared" si="0"/>
         <v>Lévêque</v>
       </c>
       <c r="D8" t="str" cm="1">
         <f t="array" aca="1" ref="D8" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>366489</v>
+        <v>879418</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Xenokrates.Lévêque@clinica.com.br</v>
       </c>
       <c r="G8" t="s">
@@ -2956,8 +3097,8 @@
         <v>6</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Xenokrates;Lévêque;366489;Xenokrates.Lévêque@clinica.com.br;Consultorio Sorriso Maroto</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Xenokrates;Lévêque;879418;Xenokrates.Lévêque@clinica.com.br;Consultorio Sorriso Maroto</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2965,19 +3106,19 @@
         <v>180</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Sandeep</v>
       </c>
       <c r="C9" t="str">
-        <f>RIGHT(A9,LEN(A9)-FIND(" ",A9,1))</f>
+        <f t="shared" si="0"/>
         <v>Schuster</v>
       </c>
       <c r="D9" t="str" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>393535</v>
+        <v>320890</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Sandeep.Schuster@clinica.com.br</v>
       </c>
       <c r="G9" t="s">
@@ -2987,8 +3128,8 @@
         <v>7</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Sandeep;Schuster;393535;Sandeep.Schuster@clinica.com.br;Clinica Marota</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Sandeep;Schuster;320890;Sandeep.Schuster@clinica.com.br;Clinica Marota</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2996,19 +3137,19 @@
         <v>181</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Naveen</v>
       </c>
       <c r="C10" t="str">
-        <f>RIGHT(A10,LEN(A10)-FIND(" ",A10,1))</f>
+        <f t="shared" si="0"/>
         <v>Mah</v>
       </c>
       <c r="D10" t="str" cm="1">
         <f t="array" aca="1" ref="D10" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>523729</v>
+        <v>390551</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Naveen.Mah@clinica.com.br</v>
       </c>
       <c r="G10" t="s">
@@ -3018,8 +3159,8 @@
         <v>8</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Naveen;Mah;523729;Naveen.Mah@clinica.com.br;Consultorio Sorriso Branquinho</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Naveen;Mah;390551;Naveen.Mah@clinica.com.br;Consultorio Sorriso Branquinho</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -3027,19 +3168,19 @@
         <v>182</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Ghayth</v>
       </c>
       <c r="C11" t="str">
-        <f>RIGHT(A11,LEN(A11)-FIND(" ",A11,1))</f>
+        <f t="shared" si="0"/>
         <v>Nifterick</v>
       </c>
       <c r="D11" t="str" cm="1">
         <f t="array" aca="1" ref="D11" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>680508</v>
+        <v>662275</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Ghayth.Nifterick@clinica.com.br</v>
       </c>
       <c r="G11" t="s">
@@ -3049,8 +3190,8 @@
         <v>9</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Ghayth;Nifterick;680508;Ghayth.Nifterick@clinica.com.br;Clinica Legal</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Ghayth;Nifterick;662275;Ghayth.Nifterick@clinica.com.br;Clinica Legal</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -3058,19 +3199,19 @@
         <v>183</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Urbanus</v>
       </c>
       <c r="C12" t="str">
-        <f>RIGHT(A12,LEN(A12)-FIND(" ",A12,1))</f>
+        <f t="shared" si="0"/>
         <v>Whitney</v>
       </c>
       <c r="D12" t="str" cm="1">
         <f t="array" aca="1" ref="D12" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>027292</v>
+        <v>551021</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Urbanus.Whitney@clinica.com.br</v>
       </c>
       <c r="G12" t="s">
@@ -3078,8 +3219,8 @@
       </c>
       <c r="I12" s="6"/>
       <c r="J12" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Urbanus;Whitney;027292;Urbanus.Whitney@clinica.com.br;Consultorio Dentes Brilhantes</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Urbanus;Whitney;551021;Urbanus.Whitney@clinica.com.br;Consultorio Dentes Brilhantes</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3087,27 +3228,27 @@
         <v>184</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Theophylaktos</v>
       </c>
       <c r="C13" t="str">
-        <f>RIGHT(A13,LEN(A13)-FIND(" ",A13,1))</f>
+        <f t="shared" si="0"/>
         <v>McCarthy</v>
       </c>
       <c r="D13" t="str" cm="1">
         <f t="array" aca="1" ref="D13" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>084181</v>
+        <v>107608</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Theophylaktos.McCarthy@clinica.com.br</v>
       </c>
       <c r="G13" t="s">
         <v>130</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Theophylaktos;McCarthy;084181;Theophylaktos.McCarthy@clinica.com.br;Clinica Da Avenida</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Theophylaktos;McCarthy;107608;Theophylaktos.McCarthy@clinica.com.br;Clinica Da Avenida</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3115,27 +3256,27 @@
         <v>185</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Abidemi</v>
       </c>
       <c r="C14" t="str">
-        <f>RIGHT(A14,LEN(A14)-FIND(" ",A14,1))</f>
+        <f t="shared" si="0"/>
         <v>D'Ambrosio</v>
       </c>
       <c r="D14" t="str" cm="1">
         <f t="array" aca="1" ref="D14" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>879341</v>
+        <v>286540</v>
       </c>
       <c r="F14" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Abidemi.D'Ambrosio@clinica.com.br</v>
       </c>
       <c r="G14" t="s">
         <v>131</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Abidemi;D'Ambrosio;879341;Abidemi.D'Ambrosio@clinica.com.br;Consultorio Sorriso Contagiante</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Abidemi;D'Ambrosio;286540;Abidemi.D'Ambrosio@clinica.com.br;Consultorio Sorriso Contagiante</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3143,27 +3284,27 @@
         <v>186</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Sohail</v>
       </c>
       <c r="C15" t="str">
-        <f>RIGHT(A15,LEN(A15)-FIND(" ",A15,1))</f>
+        <f t="shared" si="0"/>
         <v>Genovese</v>
       </c>
       <c r="D15" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>363053</v>
+        <v>986948</v>
       </c>
       <c r="F15" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Sohail.Genovese@clinica.com.br</v>
       </c>
       <c r="G15" t="s">
         <v>132</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Sohail;Genovese;363053;Sohail.Genovese@clinica.com.br;Clinica Popular</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Sohail;Genovese;986948;Sohail.Genovese@clinica.com.br;Clinica Popular</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3171,27 +3312,27 @@
         <v>187</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Apoorva</v>
       </c>
       <c r="C16" t="str">
-        <f>RIGHT(A16,LEN(A16)-FIND(" ",A16,1))</f>
+        <f t="shared" si="0"/>
         <v>Láník</v>
       </c>
       <c r="D16" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>622949</v>
+        <v>220148</v>
       </c>
       <c r="F16" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Apoorva.Láník@clinica.com.br</v>
       </c>
       <c r="G16" t="s">
         <v>133</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Apoorva;Láník;622949;Apoorva.Láník@clinica.com.br;Consultorio Saudente</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Apoorva;Láník;220148;Apoorva.Láník@clinica.com.br;Consultorio Saudente</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3199,27 +3340,27 @@
         <v>188</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Safa</v>
       </c>
       <c r="C17" t="str">
-        <f>RIGHT(A17,LEN(A17)-FIND(" ",A17,1))</f>
+        <f t="shared" si="0"/>
         <v>Eliasson</v>
       </c>
       <c r="D17" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>155593</v>
+        <v>495142</v>
       </c>
       <c r="F17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Safa.Eliasson@clinica.com.br</v>
       </c>
       <c r="G17" t="s">
         <v>135</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Safa;Eliasson;155593;Safa.Eliasson@clinica.com.br;Clinica Mega Popular</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Safa;Eliasson;495142;Safa.Eliasson@clinica.com.br;Clinica Mega Popular</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3227,27 +3368,27 @@
         <v>189</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Dudda</v>
       </c>
       <c r="C18" t="str">
-        <f>RIGHT(A18,LEN(A18)-FIND(" ",A18,1))</f>
+        <f t="shared" si="0"/>
         <v>Escamilla</v>
       </c>
       <c r="D18" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>145003</v>
+        <v>261098</v>
       </c>
       <c r="F18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Dudda.Escamilla@clinica.com.br</v>
       </c>
       <c r="G18" t="s">
         <v>120</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Dudda;Escamilla;145003;Dudda.Escamilla@clinica.com.br;Consultorio Sorisso Feliz</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Dudda;Escamilla;261098;Dudda.Escamilla@clinica.com.br;Consultorio Sorisso Feliz</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3255,27 +3396,27 @@
         <v>190</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Shyam</v>
       </c>
       <c r="C19" t="str">
-        <f>RIGHT(A19,LEN(A19)-FIND(" ",A19,1))</f>
+        <f t="shared" si="0"/>
         <v>Norup</v>
       </c>
       <c r="D19" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>696430</v>
+        <v>961651</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Shyam.Norup@clinica.com.br</v>
       </c>
       <c r="G19" t="s">
         <v>121</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Shyam;Norup;696430;Shyam.Norup@clinica.com.br;Clinica Joseph Climber</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Shyam;Norup;961651;Shyam.Norup@clinica.com.br;Clinica Joseph Climber</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3283,27 +3424,27 @@
         <v>191</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Govinda</v>
       </c>
       <c r="C20" t="str">
-        <f>RIGHT(A20,LEN(A20)-FIND(" ",A20,1))</f>
+        <f t="shared" si="0"/>
         <v>Constantin</v>
       </c>
       <c r="D20" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>212291</v>
+        <v>453087</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Govinda.Constantin@clinica.com.br</v>
       </c>
       <c r="G20" t="s">
         <v>122</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Govinda;Constantin;212291;Govinda.Constantin@clinica.com.br;Consultorio Dentes Brilhantes</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Govinda;Constantin;453087;Govinda.Constantin@clinica.com.br;Consultorio Dentes Brilhantes</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3311,27 +3452,27 @@
         <v>193</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Matej</v>
       </c>
       <c r="C21" t="str">
-        <f t="shared" ref="C21:C25" si="3">RIGHT(A21,LEN(A21)-FIND(" ",A21,1))</f>
+        <f t="shared" ref="C21:C25" si="4">RIGHT(A21,LEN(A21)-FIND(" ",A21,1))</f>
         <v>Antonescu</v>
       </c>
       <c r="D21" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>860443</v>
+        <v>834154</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Matej.Antonescu@clinica.com.br</v>
       </c>
       <c r="G21" t="s">
         <v>123</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Matej;Antonescu;860443;Matej.Antonescu@clinica.com.br;Clinica do Manuel</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Matej;Antonescu;834154;Matej.Antonescu@clinica.com.br;Clinica do Manuel</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3339,27 +3480,27 @@
         <v>194</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Zevulun</v>
       </c>
       <c r="C22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Greer</v>
       </c>
       <c r="D22" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>620938</v>
+        <v>526135</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Zevulun.Greer@clinica.com.br</v>
       </c>
       <c r="G22" t="s">
         <v>124</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Zevulun;Greer;620938;Zevulun.Greer@clinica.com.br;Consultorio Sorridente</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Zevulun;Greer;526135;Zevulun.Greer@clinica.com.br;Consultorio Sorridente</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3367,27 +3508,27 @@
         <v>195</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Elbert</v>
       </c>
       <c r="C23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Coburn</v>
       </c>
       <c r="D23" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>756846</v>
+        <v>202779</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Elbert.Coburn@clinica.com.br</v>
       </c>
       <c r="G23" t="s">
         <v>125</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Elbert;Coburn;756846;Elbert.Coburn@clinica.com.br;Clinica da Esquina</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Elbert;Coburn;202779;Elbert.Coburn@clinica.com.br;Clinica da Esquina</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3395,27 +3536,27 @@
         <v>196</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Gilad</v>
       </c>
       <c r="C24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Mehmedović</v>
       </c>
       <c r="D24" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>526330</v>
+        <v>877132</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Gilad.Mehmedović@clinica.com.br</v>
       </c>
       <c r="G24" t="s">
         <v>126</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Gilad;Mehmedović;526330;Gilad.Mehmedović@clinica.com.br;Consultorio Sorriso Maroto</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Gilad;Mehmedović;877132;Gilad.Mehmedović@clinica.com.br;Consultorio Sorriso Maroto</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3423,27 +3564,830 @@
         <v>197</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>Branko</v>
       </c>
       <c r="C25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>Hansen</v>
       </c>
       <c r="D25" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">_xlfn.TEXTJOIN("",1,INDEX($I$2:$I$11,_xlfn.RANDARRAY(6,1,1,10,TRUE)))</f>
-        <v>923147</v>
+        <v>219110</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Branko.Hansen@clinica.com.br</v>
       </c>
       <c r="G25" t="s">
         <v>127</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v>Branko;Hansen;923147;Branko.Hansen@clinica.com.br;Clinica Marota</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>Branko;Hansen;219110;Branko.Hansen@clinica.com.br;Clinica Marota</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C53DCC9-AD5B-40D3-9E8D-BE84CF0C8B3E}">
+  <dimension ref="A2:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" t="s">
+        <v>222</v>
+      </c>
+      <c r="E2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" t="s">
+        <v>171</v>
+      </c>
+      <c r="H2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;E3</f>
+        <v>Alexandre;Pedro;12335469841;12136548</v>
+      </c>
+      <c r="B3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3">
+        <v>12335469841</v>
+      </c>
+      <c r="E3">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A18" si="0">B4&amp;";"&amp;C4&amp;";"&amp;D4&amp;";"&amp;E4</f>
+        <v>Fabio;Neres;12335469842;12136548</v>
+      </c>
+      <c r="B4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4">
+        <v>12335469842</v>
+      </c>
+      <c r="E4">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>Sankler;Bergman;12335469843;12136548</v>
+      </c>
+      <c r="B5" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5">
+        <v>12335469843</v>
+      </c>
+      <c r="E5">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>Tiago;Pereira;12335469844;12136548</v>
+      </c>
+      <c r="B6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C6" t="s">
+        <v>232</v>
+      </c>
+      <c r="D6">
+        <v>12335469844</v>
+      </c>
+      <c r="E6">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>Bruno;Furukawa;12335469845;12136548</v>
+      </c>
+      <c r="B7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" t="s">
+        <v>234</v>
+      </c>
+      <c r="D7">
+        <v>12335469845</v>
+      </c>
+      <c r="E7">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>Joao;Santos;12335469846;12136548</v>
+      </c>
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D8">
+        <v>12335469846</v>
+      </c>
+      <c r="E8">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>Maria;Gasolina;12335469847;12136548</v>
+      </c>
+      <c r="B9" t="s">
+        <v>237</v>
+      </c>
+      <c r="C9" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9">
+        <v>12335469847</v>
+      </c>
+      <c r="E9">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>Joana;da Silva;12335469848;12136548</v>
+      </c>
+      <c r="B10" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" t="s">
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <v>12335469848</v>
+      </c>
+      <c r="E10">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>Jacinto;Pinto;12335469849;12136548</v>
+      </c>
+      <c r="B11" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11">
+        <v>12335469849</v>
+      </c>
+      <c r="E11">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>Miguel;Furukawa;12335469850;12136548</v>
+      </c>
+      <c r="B12" t="s">
+        <v>243</v>
+      </c>
+      <c r="C12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D12">
+        <v>12335469850</v>
+      </c>
+      <c r="E12">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>Artur;Norberto;12335469851;12136548</v>
+      </c>
+      <c r="B13" t="s">
+        <v>244</v>
+      </c>
+      <c r="C13" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13">
+        <v>12335469851</v>
+      </c>
+      <c r="E13">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>Jurema;Silva;12335469852;12136548</v>
+      </c>
+      <c r="B14" t="s">
+        <v>246</v>
+      </c>
+      <c r="C14" t="s">
+        <v>247</v>
+      </c>
+      <c r="D14">
+        <v>12335469852</v>
+      </c>
+      <c r="E14">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>Bernardo;Cornwell;12335469853;12136548</v>
+      </c>
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C15" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15">
+        <v>12335469853</v>
+      </c>
+      <c r="E15">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>Josefina;Mata;12335469854;12136548</v>
+      </c>
+      <c r="B16" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16">
+        <v>12335469854</v>
+      </c>
+      <c r="E16">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>Carlos;Joao;12335469855;12136548</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C17" t="s">
+        <v>235</v>
+      </c>
+      <c r="D17">
+        <v>12335469855</v>
+      </c>
+      <c r="E17">
+        <v>12136548</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>Marta;Maria;12335469855;12136548</v>
+      </c>
+      <c r="B18" t="s">
+        <v>253</v>
+      </c>
+      <c r="C18" t="s">
+        <v>237</v>
+      </c>
+      <c r="D18">
+        <v>12335469855</v>
+      </c>
+      <c r="E18">
+        <v>12136548</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD97EA4F-A59C-454A-B8C2-8C2EDDEBF708}">
+  <dimension ref="A2:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G2" t="s">
+        <v>259</v>
+      </c>
+      <c r="H2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>B3&amp;";"&amp;C3&amp;";"&amp;D3&amp;";"&amp;E3&amp;";"&amp;F3&amp;";"&amp;G3&amp;";"&amp;H3</f>
+        <v>banguela;pendente;2022;1;1;1;1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f t="shared" ref="A4:A18" si="0">B4&amp;";"&amp;C4&amp;";"&amp;D4&amp;";"&amp;E4&amp;";"&amp;F4&amp;";"&amp;G4&amp;";"&amp;H4</f>
+        <v>dentadura;confirmada;2022;2;2;2;2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4">
+        <v>2022</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f t="shared" si="0"/>
+        <v>dor de dente;encerrada;2022;3;3;3;3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C5" t="s">
+        <v>265</v>
+      </c>
+      <c r="D5">
+        <v>2022</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f t="shared" si="0"/>
+        <v>banguela;cancelada;2022;4;4;4;4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>261</v>
+      </c>
+      <c r="C6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6">
+        <v>2022</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f t="shared" si="0"/>
+        <v>dentadura;pendente;2022;5;5;5;5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C7" t="s">
+        <v>266</v>
+      </c>
+      <c r="D7">
+        <v>2022</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="str">
+        <f t="shared" si="0"/>
+        <v>dor de dente;confirmada;2022;6;6;6;6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D8">
+        <v>2022</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f t="shared" si="0"/>
+        <v>banguela;encerrada;2022;7;7;7;7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C9" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9">
+        <v>2022</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f t="shared" si="0"/>
+        <v>dentadura;cancelada;2022;8;8;8;8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C10" t="s">
+        <v>267</v>
+      </c>
+      <c r="D10">
+        <v>2022</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="G10">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f t="shared" si="0"/>
+        <v>dor de dente;pendente;2022;9;9;9;9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11">
+        <v>2022</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f t="shared" si="0"/>
+        <v>banguela;confirmada;2022;10;10;10;10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>261</v>
+      </c>
+      <c r="C12" t="s">
+        <v>264</v>
+      </c>
+      <c r="D12">
+        <v>2022</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>10</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f t="shared" si="0"/>
+        <v>dentadura;encerrada;2022;11;11;11;11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" t="s">
+        <v>265</v>
+      </c>
+      <c r="D13">
+        <v>2022</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>11</v>
+      </c>
+      <c r="G13">
+        <v>11</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f t="shared" si="0"/>
+        <v>dor de dente;cancelada;2022;12;12;12;12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C14" t="s">
+        <v>267</v>
+      </c>
+      <c r="D14">
+        <v>2022</v>
+      </c>
+      <c r="E14">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f t="shared" si="0"/>
+        <v>banguela;pendente;2022;1;13;13;13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>261</v>
+      </c>
+      <c r="C15" t="s">
+        <v>266</v>
+      </c>
+      <c r="D15">
+        <v>2022</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f t="shared" si="0"/>
+        <v>dentadura;confirmada;2022;2;14;14;14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>262</v>
+      </c>
+      <c r="C16" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16">
+        <v>2022</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f t="shared" si="0"/>
+        <v>dor de dente;encerrada;2022;3;15;15;15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C17" t="s">
+        <v>265</v>
+      </c>
+      <c r="D17">
+        <v>2022</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f t="shared" si="0"/>
+        <v>banguela;cancelada;2022;4;16;16;16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C18" t="s">
+        <v>267</v>
+      </c>
+      <c r="D18">
+        <v>2022</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <v>16</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>